<commit_message>
update flex PCBs with suitable buffering
</commit_message>
<xml_diff>
--- a/misc/RCP2N64RGB/doc/RCP2N64RGB_BOM.xlsx
+++ b/misc/RCP2N64RGB/doc/RCP2N64RGB_BOM.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Peter\Documents\Workspaces\Git\Eigenes\n64rgb\misc\RCP2N64RGB\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Peter\Documents\Workspaces\GitHub\n64rgb\misc\RCP2N64RGB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36E4621-C22F-4EA2-B43D-70F4885148C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B0D0DA-FA12-4536-A125-92CD4F5D4AA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="3390" windowWidth="23955" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="all versions" sheetId="10" r:id="rId1"/>
+    <sheet name="v20200705" sheetId="10" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Designator</t>
   </si>
@@ -72,39 +72,21 @@
     <t>Resistor Array (4x)</t>
   </si>
   <si>
-    <t>optional</t>
-  </si>
-  <si>
     <t>QTY per PCB</t>
   </si>
   <si>
     <t>No. of PCBs</t>
   </si>
   <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>RN1,RN2,RN3</t>
   </si>
   <si>
-    <t>5% acceptable</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
     <t>4x 33</t>
   </si>
   <si>
     <t>U1</t>
   </si>
   <si>
-    <t>SMD0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAY16-330J4LF </t>
-  </si>
-  <si>
     <t>SN74LVC1G17DCKR</t>
   </si>
   <si>
@@ -118,6 +100,42 @@
   </si>
   <si>
     <t>Buffer, Schmitt-Triggered, non-inverting</t>
+  </si>
+  <si>
+    <t>SMD0603</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>4x 0ohm</t>
+  </si>
+  <si>
+    <t>Either this, …</t>
+  </si>
+  <si>
+    <t>… or that for RN1-RN3</t>
+  </si>
+  <si>
+    <t>C1,C2</t>
+  </si>
+  <si>
+    <t>TSSOP20</t>
+  </si>
+  <si>
+    <t>9bit Buffer, Schmitt-Triggered, non-inverting</t>
+  </si>
+  <si>
+    <t>74VHC9151FT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BK32164M121-T </t>
+  </si>
+  <si>
+    <t>CAT16-000J4LF / CAY16-000J4LF</t>
   </si>
 </sst>
 </file>
@@ -944,7 +962,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475802BE-F98A-4FD9-B042-AE3F86EDB44E}">
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -958,7 +976,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1">
         <v>3</v>
@@ -972,7 +990,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>2</v>
@@ -992,52 +1010,53 @@
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D7" si="0">$B$1*C4</f>
+        <f t="shared" ref="D4:D8" si="0">$B$1*C4</f>
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F4"/>
       <c r="G4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5"/>
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D5" si="1">$B$1*C5</f>
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
+      <c r="E5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5"/>
       <c r="G5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B6"/>
       <c r="C6">
         <v>1</v>
       </c>
@@ -1046,54 +1065,83 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
         <v>9</v>
       </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>19</v>
+      <c r="F7" t="s">
+        <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
@@ -1146,16 +1194,15 @@
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F22" s="2"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F23" s="2"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F24" s="2"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
@@ -1170,39 +1217,44 @@
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
       <c r="F27" s="2"/>
-      <c r="H27" s="3"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
       <c r="F28" s="2"/>
       <c r="H28" s="3"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F30" s="2"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6"/>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F29" s="2"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F31" s="2"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F35" s="2"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F36" s="2"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
tiny correction (issue #7)
</commit_message>
<xml_diff>
--- a/misc/RCP2N64RGB/doc/RCP2N64RGB_BOM.xlsx
+++ b/misc/RCP2N64RGB/doc/RCP2N64RGB_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Peter\Documents\Workspaces\GitHub\n64rgb\misc\RCP2N64RGB\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B0D0DA-FA12-4536-A125-92CD4F5D4AA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0B24A1-809B-4B81-976E-BDCD63819610}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7815" yWindow="1260" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v20200705" sheetId="10" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>RN1,RN2,RN3</t>
   </si>
   <si>
-    <t>4x 33</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
@@ -136,6 +133,9 @@
   </si>
   <si>
     <t>CAT16-000J4LF / CAY16-000J4LF</t>
+  </si>
+  <si>
+    <t>4x ferrit bead</t>
   </si>
 </sst>
 </file>
@@ -1010,10 +1010,10 @@
     </row>
     <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1023,19 +1023,19 @@
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4"/>
       <c r="G4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1045,16 +1045,16 @@
         <v>3</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5"/>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6"/>
       <c r="C6">
@@ -1065,18 +1065,18 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1102,7 +1102,7 @@
         <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -1115,32 +1115,32 @@
         <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
         <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s">
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
         <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>

</xml_diff>